<commit_message>
Starting building in the orb writing stuff
</commit_message>
<xml_diff>
--- a/bchart.xlsx
+++ b/bchart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="370">
   <si>
     <t>0</t>
   </si>
@@ -22,72 +22,108 @@
     <t>0 Aries</t>
   </si>
   <si>
+    <t xml:space="preserve">0: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 1: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 2: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
     <t>3 Aries</t>
   </si>
   <si>
+    <t xml:space="preserve">3: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 4: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 5: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
     <t>6 Aries</t>
   </si>
   <si>
+    <t xml:space="preserve">6: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 7: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 8: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>9</t>
   </si>
   <si>
     <t>9 Aries</t>
   </si>
   <si>
+    <t xml:space="preserve">9: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 10: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 11: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>12</t>
   </si>
   <si>
     <t>12 Aries</t>
   </si>
   <si>
+    <t xml:space="preserve">12: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 13: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 14: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>15</t>
   </si>
   <si>
     <t>15 Aries</t>
   </si>
   <si>
+    <t xml:space="preserve">15: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 16: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 17: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>18</t>
   </si>
   <si>
     <t>18 Aries</t>
   </si>
   <si>
+    <t xml:space="preserve">18: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 19: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 20: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
     <t>21 Aries</t>
   </si>
   <si>
+    <t xml:space="preserve">21: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 22: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 23: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>24</t>
   </si>
   <si>
     <t>24 Aries</t>
   </si>
   <si>
+    <t xml:space="preserve">24: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 25: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 26: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>27</t>
   </si>
   <si>
     <t>27 Aries</t>
   </si>
   <si>
+    <t xml:space="preserve">27: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 28: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 29: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>30</t>
   </si>
   <si>
     <t>0 Taurus</t>
   </si>
   <si>
+    <t xml:space="preserve">30: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 31: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 32: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>33</t>
   </si>
   <si>
     <t>3 Taurus</t>
   </si>
   <si>
+    <t xml:space="preserve">33: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 34: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 35: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>36</t>
   </si>
   <si>
@@ -97,108 +133,162 @@
     <t xml:space="preserve">6: [Mars] </t>
   </si>
   <si>
+    <t xml:space="preserve">36: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 37: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 38: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>39</t>
   </si>
   <si>
     <t>9 Taurus</t>
   </si>
   <si>
+    <t xml:space="preserve">39: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 40: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 41: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>42</t>
   </si>
   <si>
     <t>12 Taurus</t>
   </si>
   <si>
+    <t xml:space="preserve">42: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 43: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 44: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>45</t>
   </si>
   <si>
     <t>15 Taurus</t>
   </si>
   <si>
+    <t xml:space="preserve">45: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 46: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 47: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>48</t>
   </si>
   <si>
     <t>18 Taurus</t>
   </si>
   <si>
+    <t xml:space="preserve">48: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 49: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 50: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>51</t>
   </si>
   <si>
     <t>21 Taurus</t>
   </si>
   <si>
+    <t xml:space="preserve">51: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 52: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 53: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>54</t>
   </si>
   <si>
     <t>24 Taurus</t>
   </si>
   <si>
+    <t xml:space="preserve">54: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 55: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 56: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>57</t>
   </si>
   <si>
     <t>27 Taurus</t>
   </si>
   <si>
+    <t xml:space="preserve">57: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 58: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 59: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>60</t>
   </si>
   <si>
     <t>0 Gemini</t>
   </si>
   <si>
+    <t xml:space="preserve">60: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 61: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 62: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>63</t>
   </si>
   <si>
     <t>3 Gemini</t>
   </si>
   <si>
+    <t xml:space="preserve">63: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 64: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 65: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>66</t>
   </si>
   <si>
     <t>6 Gemini</t>
   </si>
   <si>
+    <t xml:space="preserve">66: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 67: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 68: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>69</t>
   </si>
   <si>
     <t>9 Gemini</t>
   </si>
   <si>
+    <t xml:space="preserve">69: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 70: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 71: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>72</t>
   </si>
   <si>
     <t>12 Gemini</t>
   </si>
   <si>
+    <t xml:space="preserve">72: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 73: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 74: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>75</t>
   </si>
   <si>
     <t>15 Gemini</t>
   </si>
   <si>
+    <t xml:space="preserve">75: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 76: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 77: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>78</t>
   </si>
   <si>
     <t>18 Gemini</t>
   </si>
   <si>
+    <t xml:space="preserve">78: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 79: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 80: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>81</t>
   </si>
   <si>
     <t>21 Gemini</t>
   </si>
   <si>
+    <t xml:space="preserve">81: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 82: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 83: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>84</t>
   </si>
   <si>
     <t>24 Gemini</t>
   </si>
   <si>
+    <t xml:space="preserve">84: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 85: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 86: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>87</t>
   </si>
   <si>
     <t>27 Gemini</t>
   </si>
   <si>
+    <t xml:space="preserve">87: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 88: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 89: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>90</t>
   </si>
   <si>
@@ -208,90 +298,135 @@
     <t xml:space="preserve">2: [Saturn] </t>
   </si>
   <si>
+    <t xml:space="preserve">90: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 91: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 92: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>93</t>
   </si>
   <si>
     <t>3 Cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">93: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 94: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 95: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>96</t>
   </si>
   <si>
     <t>6 Cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">96: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 97: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 98: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>99</t>
   </si>
   <si>
     <t>9 Cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">99: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 100: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 101: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>102</t>
   </si>
   <si>
     <t>12 Cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">102: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 103: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 104: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>105</t>
   </si>
   <si>
     <t>15 Cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">105: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 106: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 107: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>108</t>
   </si>
   <si>
     <t>18 Cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">108: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 109: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 110: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>111</t>
   </si>
   <si>
     <t>21 Cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">111: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 112: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 113: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>114</t>
   </si>
   <si>
     <t>24 Cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">114: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 115: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 116: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>117</t>
   </si>
   <si>
     <t>27 Cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">117: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 118: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 119: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>120</t>
   </si>
   <si>
     <t>0 Leo</t>
   </si>
   <si>
+    <t xml:space="preserve">120: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 121: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 122: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>123</t>
   </si>
   <si>
     <t>3 Leo</t>
   </si>
   <si>
+    <t xml:space="preserve">123: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 124: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 125: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>126</t>
   </si>
   <si>
     <t>6 Leo</t>
   </si>
   <si>
+    <t xml:space="preserve">126: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 127: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 128: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>129</t>
   </si>
   <si>
     <t>9 Leo</t>
   </si>
   <si>
+    <t xml:space="preserve">129: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 130: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 131: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>132</t>
   </si>
   <si>
     <t>12 Leo</t>
   </si>
   <si>
+    <t xml:space="preserve">132: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 133: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 134: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>135</t>
   </si>
   <si>
@@ -301,42 +436,63 @@
     <t xml:space="preserve">17: [Asc] </t>
   </si>
   <si>
+    <t xml:space="preserve">135: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 136: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 137: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>138</t>
   </si>
   <si>
     <t>18 Leo</t>
   </si>
   <si>
+    <t xml:space="preserve">138: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 139: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 140: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>141</t>
   </si>
   <si>
     <t>21 Leo</t>
   </si>
   <si>
+    <t xml:space="preserve">141: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 142: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 143: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>144</t>
   </si>
   <si>
     <t>24 Leo</t>
   </si>
   <si>
+    <t xml:space="preserve">144: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 145: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 146: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>147</t>
   </si>
   <si>
     <t>27 Leo</t>
   </si>
   <si>
+    <t xml:space="preserve">147: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 148: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 149: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>150</t>
   </si>
   <si>
     <t>0 Virgo</t>
   </si>
   <si>
+    <t xml:space="preserve">150: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 151: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 152: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>153</t>
   </si>
   <si>
     <t>3 Virgo</t>
   </si>
   <si>
+    <t xml:space="preserve">153: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 154: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 155: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>156</t>
   </si>
   <si>
@@ -346,54 +502,81 @@
     <t xml:space="preserve">7: [Mercury] 8: [Sun] </t>
   </si>
   <si>
+    <t xml:space="preserve">156: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 157: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 158: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>159</t>
   </si>
   <si>
     <t>9 Virgo</t>
   </si>
   <si>
+    <t xml:space="preserve">159: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 160: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 161: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>162</t>
   </si>
   <si>
     <t>12 Virgo</t>
   </si>
   <si>
+    <t xml:space="preserve">162: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 163: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 164: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>165</t>
   </si>
   <si>
     <t>15 Virgo</t>
   </si>
   <si>
+    <t xml:space="preserve">165: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 166: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 167: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>168</t>
   </si>
   <si>
     <t>18 Virgo</t>
   </si>
   <si>
+    <t xml:space="preserve">168: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 169: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 170: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>171</t>
   </si>
   <si>
     <t>21 Virgo</t>
   </si>
   <si>
+    <t xml:space="preserve">171: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 172: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 173: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>174</t>
   </si>
   <si>
     <t>24 Virgo</t>
   </si>
   <si>
+    <t xml:space="preserve">174: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 175: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 176: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>177</t>
   </si>
   <si>
     <t>27 Virgo</t>
   </si>
   <si>
+    <t xml:space="preserve">177: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 178: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 179: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>180</t>
   </si>
   <si>
     <t>0 Libra</t>
   </si>
   <si>
+    <t xml:space="preserve">180: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 181: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 182: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>183</t>
   </si>
   <si>
@@ -403,24 +586,36 @@
     <t xml:space="preserve">3: [Pluto] </t>
   </si>
   <si>
+    <t xml:space="preserve">183: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 184: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 185: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>186</t>
   </si>
   <si>
     <t>6 Libra</t>
   </si>
   <si>
+    <t xml:space="preserve">186: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 187: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 188: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>189</t>
   </si>
   <si>
     <t>9 Libra</t>
   </si>
   <si>
+    <t xml:space="preserve">189: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 190: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 191: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>192</t>
   </si>
   <si>
     <t>12 Libra</t>
   </si>
   <si>
+    <t xml:space="preserve">192: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 193: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 194: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>195</t>
   </si>
   <si>
@@ -430,6 +625,9 @@
     <t xml:space="preserve">15: [Venus] </t>
   </si>
   <si>
+    <t xml:space="preserve">195: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 196: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 197: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>198</t>
   </si>
   <si>
@@ -439,24 +637,36 @@
     <t xml:space="preserve">20: [Uranus] </t>
   </si>
   <si>
+    <t xml:space="preserve">198: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 199: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 200: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>201</t>
   </si>
   <si>
     <t>21 Libra</t>
   </si>
   <si>
+    <t xml:space="preserve">201: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 202: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 203: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>204</t>
   </si>
   <si>
     <t>24 Libra</t>
   </si>
   <si>
+    <t xml:space="preserve">204: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 205: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 206: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>207</t>
   </si>
   <si>
     <t>27 Libra</t>
   </si>
   <si>
+    <t xml:space="preserve">207: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 208: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 209: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>210</t>
   </si>
   <si>
@@ -466,66 +676,99 @@
     <t xml:space="preserve">2: [Moon] </t>
   </si>
   <si>
+    <t xml:space="preserve">210: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 211: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 212: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>213</t>
   </si>
   <si>
     <t>3 Scorpio</t>
   </si>
   <si>
+    <t xml:space="preserve">213: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 214: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 215: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>216</t>
   </si>
   <si>
     <t>6 Scorpio</t>
   </si>
   <si>
+    <t xml:space="preserve">216: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 217: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 218: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>219</t>
   </si>
   <si>
     <t>9 Scorpio</t>
   </si>
   <si>
+    <t xml:space="preserve">219: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 220: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 221: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>222</t>
   </si>
   <si>
     <t>12 Scorpio</t>
   </si>
   <si>
+    <t xml:space="preserve">222: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 223: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 224: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>225</t>
   </si>
   <si>
     <t>15 Scorpio</t>
   </si>
   <si>
+    <t xml:space="preserve">225: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 226: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 227: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>228</t>
   </si>
   <si>
     <t>18 Scorpio</t>
   </si>
   <si>
+    <t xml:space="preserve">228: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 229: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 230: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>231</t>
   </si>
   <si>
     <t>21 Scorpio</t>
   </si>
   <si>
+    <t xml:space="preserve">231: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 232: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 233: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>234</t>
   </si>
   <si>
     <t>24 Scorpio</t>
   </si>
   <si>
+    <t xml:space="preserve">234: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 235: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 236: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>237</t>
   </si>
   <si>
     <t>27 Scorpio</t>
   </si>
   <si>
+    <t xml:space="preserve">237: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 238: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 239: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>240</t>
   </si>
   <si>
     <t>0 Sagitarrius</t>
   </si>
   <si>
+    <t xml:space="preserve">240: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 241: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 242: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>243</t>
   </si>
   <si>
@@ -535,120 +778,180 @@
     <t xml:space="preserve">4: [Neptune] </t>
   </si>
   <si>
+    <t xml:space="preserve">243: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 244: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 245: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>246</t>
   </si>
   <si>
     <t>6 Sagitarrius</t>
   </si>
   <si>
+    <t xml:space="preserve">246: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 247: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 248: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>249</t>
   </si>
   <si>
     <t>9 Sagitarrius</t>
   </si>
   <si>
+    <t xml:space="preserve">249: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 250: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 251: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>252</t>
   </si>
   <si>
     <t>12 Sagitarrius</t>
   </si>
   <si>
+    <t xml:space="preserve">252: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 253: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 254: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>255</t>
   </si>
   <si>
     <t>15 Sagitarrius</t>
   </si>
   <si>
+    <t xml:space="preserve">255: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 256: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 257: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>258</t>
   </si>
   <si>
     <t>18 Sagitarrius</t>
   </si>
   <si>
+    <t xml:space="preserve">258: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 259: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 260: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>261</t>
   </si>
   <si>
     <t>21 Sagitarrius</t>
   </si>
   <si>
+    <t xml:space="preserve">261: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 262: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 263: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>264</t>
   </si>
   <si>
     <t>24 Sagitarrius</t>
   </si>
   <si>
+    <t xml:space="preserve">264: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 265: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 266: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>267</t>
   </si>
   <si>
     <t>27 Sagitarrius</t>
   </si>
   <si>
+    <t xml:space="preserve">267: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 268: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 269: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>270</t>
   </si>
   <si>
     <t>0 Capricorn</t>
   </si>
   <si>
+    <t xml:space="preserve">270: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 271: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 272: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>273</t>
   </si>
   <si>
     <t>3 Capricorn</t>
   </si>
   <si>
+    <t xml:space="preserve">273: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 274: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 275: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>276</t>
   </si>
   <si>
     <t>6 Capricorn</t>
   </si>
   <si>
+    <t xml:space="preserve">276: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 277: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 278: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>279</t>
   </si>
   <si>
     <t>9 Capricorn</t>
   </si>
   <si>
+    <t xml:space="preserve">279: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 280: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 281: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>282</t>
   </si>
   <si>
     <t>12 Capricorn</t>
   </si>
   <si>
+    <t xml:space="preserve">282: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 283: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 284: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>285</t>
   </si>
   <si>
     <t>15 Capricorn</t>
   </si>
   <si>
+    <t xml:space="preserve">285: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 286: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 287: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>288</t>
   </si>
   <si>
     <t>18 Capricorn</t>
   </si>
   <si>
+    <t xml:space="preserve">288: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 289: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 290: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>291</t>
   </si>
   <si>
     <t>21 Capricorn</t>
   </si>
   <si>
+    <t xml:space="preserve">291: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 292: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 293: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>294</t>
   </si>
   <si>
     <t>24 Capricorn</t>
   </si>
   <si>
+    <t xml:space="preserve">294: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 295: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 296: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>297</t>
   </si>
   <si>
     <t>27 Capricorn</t>
   </si>
   <si>
+    <t xml:space="preserve">297: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 298: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 299: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>300</t>
   </si>
   <si>
     <t>0 Aquarius</t>
   </si>
   <si>
+    <t xml:space="preserve">300: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 301: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 302: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>303</t>
   </si>
   <si>
@@ -658,112 +961,169 @@
     <t xml:space="preserve">3: [Jupiter] </t>
   </si>
   <si>
+    <t xml:space="preserve">303: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 304: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 305: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>306</t>
   </si>
   <si>
     <t>6 Aquarius</t>
   </si>
   <si>
+    <t xml:space="preserve">306: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 307: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 308: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>309</t>
   </si>
   <si>
     <t>9 Aquarius</t>
   </si>
   <si>
+    <t xml:space="preserve">309: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 310: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 311: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>312</t>
   </si>
   <si>
     <t>12 Aquarius</t>
   </si>
   <si>
+    <t xml:space="preserve">312: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 313: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 314: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>315</t>
   </si>
   <si>
     <t>15 Aquarius</t>
   </si>
   <si>
+    <t xml:space="preserve">315: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 316: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 317: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>318</t>
   </si>
   <si>
     <t>18 Aquarius</t>
   </si>
   <si>
+    <t xml:space="preserve">318: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 319: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 320: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>321</t>
   </si>
   <si>
     <t>21 Aquarius</t>
   </si>
   <si>
+    <t xml:space="preserve">321: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 322: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 323: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>324</t>
   </si>
   <si>
     <t>24 Aquarius</t>
   </si>
   <si>
+    <t xml:space="preserve">324: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 325: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 326: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>327</t>
   </si>
   <si>
     <t>27 Aquarius</t>
   </si>
   <si>
+    <t xml:space="preserve">327: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 328: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 329: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>330</t>
   </si>
   <si>
     <t>0 Pisces</t>
   </si>
   <si>
+    <t xml:space="preserve">330: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 331: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 332: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>333</t>
   </si>
   <si>
     <t>3 Pisces</t>
   </si>
   <si>
+    <t xml:space="preserve">333: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 334: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 335: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>336</t>
   </si>
   <si>
     <t>6 Pisces</t>
   </si>
   <si>
+    <t xml:space="preserve">336: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 337: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 338: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>339</t>
   </si>
   <si>
     <t>9 Pisces</t>
   </si>
   <si>
+    <t xml:space="preserve">339: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 340: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 341: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>342</t>
   </si>
   <si>
     <t>12 Pisces</t>
   </si>
   <si>
+    <t xml:space="preserve">342: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 343: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 344: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>345</t>
   </si>
   <si>
     <t>15 Pisces</t>
   </si>
   <si>
+    <t xml:space="preserve">345: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 346: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 347: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>348</t>
   </si>
   <si>
     <t>18 Pisces</t>
   </si>
   <si>
+    <t xml:space="preserve">348: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 349: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 350: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>351</t>
   </si>
   <si>
     <t>21 Pisces</t>
   </si>
   <si>
+    <t xml:space="preserve">351: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 352: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 353: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>354</t>
   </si>
   <si>
     <t>24 Pisces</t>
   </si>
   <si>
+    <t xml:space="preserve">354: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 355: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 356: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+  </si>
+  <si>
     <t>357</t>
   </si>
   <si>
     <t>27 Pisces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">357: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 358: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 359: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
   </si>
 </sst>
 </file>
@@ -1105,6 +1465,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -1113,985 +1476,1312 @@
       </c>
     </row>
     <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:4">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:4">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:4">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:4">
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:4">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="2:4">
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="2:4">
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:4">
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="2:4">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="2:4">
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="2:4">
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="2:4">
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="2:4">
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="2:4">
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="2:4">
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="2:4">
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="2:4">
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="2:4">
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="2:4">
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="2:4">
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="2:4">
+      <c r="B34" t="s">
+        <v>103</v>
+      </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="2:4">
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="2:4">
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="2:4">
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="2:4">
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="2:4">
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="2:4">
+      <c r="B40" t="s">
+        <v>121</v>
+      </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="2:4">
+      <c r="B41" t="s">
+        <v>124</v>
+      </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="D41" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="2:4">
+      <c r="B42" t="s">
+        <v>127</v>
+      </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="D42" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="2:4">
+      <c r="B43" t="s">
+        <v>130</v>
+      </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="D43" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="2:4">
+      <c r="B44" t="s">
+        <v>133</v>
+      </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="D44" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="2:4">
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="D45" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="2:4">
+      <c r="B47" t="s">
+        <v>143</v>
+      </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>142</v>
       </c>
       <c r="D47" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="2:4">
+      <c r="B48" t="s">
+        <v>146</v>
+      </c>
       <c r="C48" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="D48" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="2:4">
+      <c r="B49" t="s">
+        <v>149</v>
+      </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="D49" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="2:4">
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
       <c r="D50" t="s">
-        <v>101</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="2:4">
+      <c r="B51" t="s">
+        <v>155</v>
+      </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>154</v>
       </c>
       <c r="D51" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="2:4">
+      <c r="B52" t="s">
+        <v>158</v>
+      </c>
       <c r="C52" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
       <c r="D52" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" t="s">
-        <v>109</v>
+        <v>162</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D53" t="s">
-        <v>107</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="2:4">
+      <c r="B54" t="s">
+        <v>165</v>
+      </c>
       <c r="C54" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="D54" t="s">
-        <v>110</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="2:4">
+      <c r="B55" t="s">
+        <v>168</v>
+      </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="D55" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="2:4">
+      <c r="B56" t="s">
+        <v>171</v>
+      </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="D56" t="s">
-        <v>114</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="2:4">
+      <c r="B57" t="s">
+        <v>174</v>
+      </c>
       <c r="C57" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="D57" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="2:4">
+      <c r="B58" t="s">
+        <v>177</v>
+      </c>
       <c r="C58" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="D58" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="2:4">
+      <c r="B59" t="s">
+        <v>180</v>
+      </c>
       <c r="C59" t="s">
-        <v>121</v>
+        <v>179</v>
       </c>
       <c r="D59" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="2:4">
+      <c r="B60" t="s">
+        <v>183</v>
+      </c>
       <c r="C60" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="D60" t="s">
-        <v>122</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="2:4">
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
       <c r="C61" t="s">
-        <v>125</v>
+        <v>185</v>
       </c>
       <c r="D61" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="B62" t="s">
-        <v>128</v>
+        <v>190</v>
       </c>
       <c r="C62" t="s">
-        <v>127</v>
+        <v>188</v>
       </c>
       <c r="D62" t="s">
-        <v>126</v>
+        <v>187</v>
       </c>
     </row>
     <row r="63" spans="2:4">
+      <c r="B63" t="s">
+        <v>193</v>
+      </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
-        <v>129</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="2:4">
+      <c r="B64" t="s">
+        <v>196</v>
+      </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="D64" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="2:4">
+      <c r="B65" t="s">
+        <v>199</v>
+      </c>
       <c r="C65" t="s">
-        <v>134</v>
+        <v>198</v>
       </c>
       <c r="D65" t="s">
-        <v>133</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="B66" t="s">
-        <v>137</v>
+        <v>203</v>
       </c>
       <c r="C66" t="s">
-        <v>136</v>
+        <v>201</v>
       </c>
       <c r="D66" t="s">
-        <v>135</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="2:4">
       <c r="B67" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
       <c r="C67" t="s">
-        <v>139</v>
+        <v>205</v>
       </c>
       <c r="D67" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="2:4">
+      <c r="B68" t="s">
+        <v>210</v>
+      </c>
       <c r="C68" t="s">
-        <v>142</v>
+        <v>209</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="2:4">
+      <c r="B69" t="s">
+        <v>213</v>
+      </c>
       <c r="C69" t="s">
-        <v>144</v>
+        <v>212</v>
       </c>
       <c r="D69" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="2:4">
+      <c r="B70" t="s">
+        <v>216</v>
+      </c>
       <c r="C70" t="s">
-        <v>146</v>
+        <v>215</v>
       </c>
       <c r="D70" t="s">
-        <v>145</v>
+        <v>214</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="B71" t="s">
-        <v>149</v>
+        <v>220</v>
       </c>
       <c r="C71" t="s">
-        <v>148</v>
+        <v>218</v>
       </c>
       <c r="D71" t="s">
-        <v>147</v>
+        <v>217</v>
       </c>
     </row>
     <row r="72" spans="2:4">
+      <c r="B72" t="s">
+        <v>223</v>
+      </c>
       <c r="C72" t="s">
-        <v>151</v>
+        <v>222</v>
       </c>
       <c r="D72" t="s">
-        <v>150</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="2:4">
+      <c r="B73" t="s">
+        <v>226</v>
+      </c>
       <c r="C73" t="s">
-        <v>153</v>
+        <v>225</v>
       </c>
       <c r="D73" t="s">
-        <v>152</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="2:4">
+      <c r="B74" t="s">
+        <v>229</v>
+      </c>
       <c r="C74" t="s">
-        <v>155</v>
+        <v>228</v>
       </c>
       <c r="D74" t="s">
-        <v>154</v>
+        <v>227</v>
       </c>
     </row>
     <row r="75" spans="2:4">
+      <c r="B75" t="s">
+        <v>232</v>
+      </c>
       <c r="C75" t="s">
-        <v>157</v>
+        <v>231</v>
       </c>
       <c r="D75" t="s">
-        <v>156</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="2:4">
+      <c r="B76" t="s">
+        <v>235</v>
+      </c>
       <c r="C76" t="s">
-        <v>159</v>
+        <v>234</v>
       </c>
       <c r="D76" t="s">
-        <v>158</v>
+        <v>233</v>
       </c>
     </row>
     <row r="77" spans="2:4">
+      <c r="B77" t="s">
+        <v>238</v>
+      </c>
       <c r="C77" t="s">
-        <v>161</v>
+        <v>237</v>
       </c>
       <c r="D77" t="s">
-        <v>160</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="2:4">
+      <c r="B78" t="s">
+        <v>241</v>
+      </c>
       <c r="C78" t="s">
-        <v>163</v>
+        <v>240</v>
       </c>
       <c r="D78" t="s">
-        <v>162</v>
+        <v>239</v>
       </c>
     </row>
     <row r="79" spans="2:4">
+      <c r="B79" t="s">
+        <v>244</v>
+      </c>
       <c r="C79" t="s">
-        <v>165</v>
+        <v>243</v>
       </c>
       <c r="D79" t="s">
-        <v>164</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="2:4">
+      <c r="B80" t="s">
+        <v>247</v>
+      </c>
       <c r="C80" t="s">
-        <v>167</v>
+        <v>246</v>
       </c>
       <c r="D80" t="s">
-        <v>166</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="2:4">
+      <c r="B81" t="s">
+        <v>250</v>
+      </c>
       <c r="C81" t="s">
-        <v>169</v>
+        <v>249</v>
       </c>
       <c r="D81" t="s">
-        <v>168</v>
+        <v>248</v>
       </c>
     </row>
     <row r="82" spans="2:4">
       <c r="B82" t="s">
-        <v>172</v>
+        <v>254</v>
       </c>
       <c r="C82" t="s">
-        <v>171</v>
+        <v>252</v>
       </c>
       <c r="D82" t="s">
-        <v>170</v>
+        <v>251</v>
       </c>
     </row>
     <row r="83" spans="2:4">
+      <c r="B83" t="s">
+        <v>257</v>
+      </c>
       <c r="C83" t="s">
-        <v>174</v>
+        <v>256</v>
       </c>
       <c r="D83" t="s">
-        <v>173</v>
+        <v>255</v>
       </c>
     </row>
     <row r="84" spans="2:4">
+      <c r="B84" t="s">
+        <v>260</v>
+      </c>
       <c r="C84" t="s">
-        <v>176</v>
+        <v>259</v>
       </c>
       <c r="D84" t="s">
-        <v>175</v>
+        <v>258</v>
       </c>
     </row>
     <row r="85" spans="2:4">
+      <c r="B85" t="s">
+        <v>263</v>
+      </c>
       <c r="C85" t="s">
-        <v>178</v>
+        <v>262</v>
       </c>
       <c r="D85" t="s">
-        <v>177</v>
+        <v>261</v>
       </c>
     </row>
     <row r="86" spans="2:4">
+      <c r="B86" t="s">
+        <v>266</v>
+      </c>
       <c r="C86" t="s">
-        <v>180</v>
+        <v>265</v>
       </c>
       <c r="D86" t="s">
-        <v>179</v>
+        <v>264</v>
       </c>
     </row>
     <row r="87" spans="2:4">
+      <c r="B87" t="s">
+        <v>269</v>
+      </c>
       <c r="C87" t="s">
-        <v>182</v>
+        <v>268</v>
       </c>
       <c r="D87" t="s">
-        <v>181</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="2:4">
+      <c r="B88" t="s">
+        <v>272</v>
+      </c>
       <c r="C88" t="s">
-        <v>184</v>
+        <v>271</v>
       </c>
       <c r="D88" t="s">
-        <v>183</v>
+        <v>270</v>
       </c>
     </row>
     <row r="89" spans="2:4">
+      <c r="B89" t="s">
+        <v>275</v>
+      </c>
       <c r="C89" t="s">
-        <v>186</v>
+        <v>274</v>
       </c>
       <c r="D89" t="s">
-        <v>185</v>
+        <v>273</v>
       </c>
     </row>
     <row r="90" spans="2:4">
+      <c r="B90" t="s">
+        <v>278</v>
+      </c>
       <c r="C90" t="s">
-        <v>188</v>
+        <v>277</v>
       </c>
       <c r="D90" t="s">
-        <v>187</v>
+        <v>276</v>
       </c>
     </row>
     <row r="91" spans="2:4">
+      <c r="B91" t="s">
+        <v>281</v>
+      </c>
       <c r="C91" t="s">
-        <v>190</v>
+        <v>280</v>
       </c>
       <c r="D91" t="s">
-        <v>189</v>
+        <v>279</v>
       </c>
     </row>
     <row r="92" spans="2:4">
+      <c r="B92" t="s">
+        <v>284</v>
+      </c>
       <c r="C92" t="s">
-        <v>192</v>
+        <v>283</v>
       </c>
       <c r="D92" t="s">
-        <v>191</v>
+        <v>282</v>
       </c>
     </row>
     <row r="93" spans="2:4">
+      <c r="B93" t="s">
+        <v>287</v>
+      </c>
       <c r="C93" t="s">
-        <v>194</v>
+        <v>286</v>
       </c>
       <c r="D93" t="s">
-        <v>193</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="2:4">
+      <c r="B94" t="s">
+        <v>290</v>
+      </c>
       <c r="C94" t="s">
-        <v>196</v>
+        <v>289</v>
       </c>
       <c r="D94" t="s">
-        <v>195</v>
+        <v>288</v>
       </c>
     </row>
     <row r="95" spans="2:4">
+      <c r="B95" t="s">
+        <v>293</v>
+      </c>
       <c r="C95" t="s">
-        <v>198</v>
+        <v>292</v>
       </c>
       <c r="D95" t="s">
-        <v>197</v>
+        <v>291</v>
       </c>
     </row>
     <row r="96" spans="2:4">
+      <c r="B96" t="s">
+        <v>296</v>
+      </c>
       <c r="C96" t="s">
-        <v>200</v>
+        <v>295</v>
       </c>
       <c r="D96" t="s">
-        <v>199</v>
+        <v>294</v>
       </c>
     </row>
     <row r="97" spans="2:4">
+      <c r="B97" t="s">
+        <v>299</v>
+      </c>
       <c r="C97" t="s">
-        <v>202</v>
+        <v>298</v>
       </c>
       <c r="D97" t="s">
-        <v>201</v>
+        <v>297</v>
       </c>
     </row>
     <row r="98" spans="2:4">
+      <c r="B98" t="s">
+        <v>302</v>
+      </c>
       <c r="C98" t="s">
-        <v>204</v>
+        <v>301</v>
       </c>
       <c r="D98" t="s">
-        <v>203</v>
+        <v>300</v>
       </c>
     </row>
     <row r="99" spans="2:4">
+      <c r="B99" t="s">
+        <v>305</v>
+      </c>
       <c r="C99" t="s">
-        <v>206</v>
+        <v>304</v>
       </c>
       <c r="D99" t="s">
-        <v>205</v>
+        <v>303</v>
       </c>
     </row>
     <row r="100" spans="2:4">
+      <c r="B100" t="s">
+        <v>308</v>
+      </c>
       <c r="C100" t="s">
-        <v>208</v>
+        <v>307</v>
       </c>
       <c r="D100" t="s">
-        <v>207</v>
+        <v>306</v>
       </c>
     </row>
     <row r="101" spans="2:4">
+      <c r="B101" t="s">
+        <v>311</v>
+      </c>
       <c r="C101" t="s">
-        <v>210</v>
+        <v>310</v>
       </c>
       <c r="D101" t="s">
-        <v>209</v>
+        <v>309</v>
       </c>
     </row>
     <row r="102" spans="2:4">
       <c r="B102" t="s">
-        <v>213</v>
+        <v>315</v>
       </c>
       <c r="C102" t="s">
-        <v>212</v>
+        <v>313</v>
       </c>
       <c r="D102" t="s">
-        <v>211</v>
+        <v>312</v>
       </c>
     </row>
     <row r="103" spans="2:4">
+      <c r="B103" t="s">
+        <v>318</v>
+      </c>
       <c r="C103" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="D103" t="s">
-        <v>214</v>
+        <v>316</v>
       </c>
     </row>
     <row r="104" spans="2:4">
+      <c r="B104" t="s">
+        <v>321</v>
+      </c>
       <c r="C104" t="s">
-        <v>217</v>
+        <v>320</v>
       </c>
       <c r="D104" t="s">
-        <v>216</v>
+        <v>319</v>
       </c>
     </row>
     <row r="105" spans="2:4">
+      <c r="B105" t="s">
+        <v>324</v>
+      </c>
       <c r="C105" t="s">
-        <v>219</v>
+        <v>323</v>
       </c>
       <c r="D105" t="s">
-        <v>218</v>
+        <v>322</v>
       </c>
     </row>
     <row r="106" spans="2:4">
+      <c r="B106" t="s">
+        <v>327</v>
+      </c>
       <c r="C106" t="s">
-        <v>221</v>
+        <v>326</v>
       </c>
       <c r="D106" t="s">
-        <v>220</v>
+        <v>325</v>
       </c>
     </row>
     <row r="107" spans="2:4">
+      <c r="B107" t="s">
+        <v>330</v>
+      </c>
       <c r="C107" t="s">
-        <v>223</v>
+        <v>329</v>
       </c>
       <c r="D107" t="s">
-        <v>222</v>
+        <v>328</v>
       </c>
     </row>
     <row r="108" spans="2:4">
+      <c r="B108" t="s">
+        <v>333</v>
+      </c>
       <c r="C108" t="s">
-        <v>225</v>
+        <v>332</v>
       </c>
       <c r="D108" t="s">
-        <v>224</v>
+        <v>331</v>
       </c>
     </row>
     <row r="109" spans="2:4">
+      <c r="B109" t="s">
+        <v>336</v>
+      </c>
       <c r="C109" t="s">
-        <v>227</v>
+        <v>335</v>
       </c>
       <c r="D109" t="s">
-        <v>226</v>
+        <v>334</v>
       </c>
     </row>
     <row r="110" spans="2:4">
+      <c r="B110" t="s">
+        <v>339</v>
+      </c>
       <c r="C110" t="s">
-        <v>229</v>
+        <v>338</v>
       </c>
       <c r="D110" t="s">
-        <v>228</v>
+        <v>337</v>
       </c>
     </row>
     <row r="111" spans="2:4">
+      <c r="B111" t="s">
+        <v>342</v>
+      </c>
       <c r="C111" t="s">
-        <v>231</v>
+        <v>341</v>
       </c>
       <c r="D111" t="s">
-        <v>230</v>
+        <v>340</v>
       </c>
     </row>
     <row r="112" spans="2:4">
+      <c r="B112" t="s">
+        <v>345</v>
+      </c>
       <c r="C112" t="s">
-        <v>233</v>
+        <v>344</v>
       </c>
       <c r="D112" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="113" spans="3:4">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4">
+      <c r="B113" t="s">
+        <v>348</v>
+      </c>
       <c r="C113" t="s">
-        <v>235</v>
+        <v>347</v>
       </c>
       <c r="D113" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="114" spans="3:4">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4">
+      <c r="B114" t="s">
+        <v>351</v>
+      </c>
       <c r="C114" t="s">
-        <v>237</v>
+        <v>350</v>
       </c>
       <c r="D114" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="115" spans="3:4">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4">
+      <c r="B115" t="s">
+        <v>354</v>
+      </c>
       <c r="C115" t="s">
-        <v>239</v>
+        <v>353</v>
       </c>
       <c r="D115" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="116" spans="3:4">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4">
+      <c r="B116" t="s">
+        <v>357</v>
+      </c>
       <c r="C116" t="s">
-        <v>241</v>
+        <v>356</v>
       </c>
       <c r="D116" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="117" spans="3:4">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4">
+      <c r="B117" t="s">
+        <v>360</v>
+      </c>
       <c r="C117" t="s">
-        <v>243</v>
+        <v>359</v>
       </c>
       <c r="D117" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="118" spans="3:4">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4">
+      <c r="B118" t="s">
+        <v>363</v>
+      </c>
       <c r="C118" t="s">
-        <v>245</v>
+        <v>362</v>
       </c>
       <c r="D118" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="119" spans="3:4">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4">
+      <c r="B119" t="s">
+        <v>366</v>
+      </c>
       <c r="C119" t="s">
-        <v>247</v>
+        <v>365</v>
       </c>
       <c r="D119" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="120" spans="3:4">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4">
+      <c r="B120" t="s">
+        <v>369</v>
+      </c>
       <c r="C120" t="s">
-        <v>249</v>
+        <v>368</v>
       </c>
       <c r="D120" t="s">
-        <v>248</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put the aspects into the chart
</commit_message>
<xml_diff>
--- a/bchart.xlsx
+++ b/bchart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="329">
   <si>
     <t>0</t>
   </si>
@@ -22,16 +22,13 @@
     <t>0 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">0: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 1: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 2: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
     <t>3 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">3: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 4: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 5: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">5: [Venus Opposition] </t>
   </si>
   <si>
     <t>6</t>
@@ -40,16 +37,13 @@
     <t>6 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">6: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 7: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 8: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
     <t>9 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">9: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 10: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 11: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">9: [Jupiter Sextile] 10: [Uranus Opposition] 11: [Moon Quincunx] </t>
   </si>
   <si>
     <t>12</t>
@@ -58,7 +52,7 @@
     <t>12 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">12: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 13: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 14: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">12: [Neptune Trine] 13: [Pluto Opposition] </t>
   </si>
   <si>
     <t>15</t>
@@ -67,25 +61,19 @@
     <t>15 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">15: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 16: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 17: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
     <t>18 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">18: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 19: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 20: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
     <t>21 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">21: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 22: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 23: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">23: [Moon Opposition] </t>
   </si>
   <si>
     <t>24</t>
@@ -94,7 +82,7 @@
     <t>24 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">24: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 25: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 26: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">25: [Venus Opposition Jupiter Square] 26: [Mars Conj] </t>
   </si>
   <si>
     <t>27</t>
@@ -103,16 +91,13 @@
     <t>27 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">27: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 28: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 29: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
     <t>0 Taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">30: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 31: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 32: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">30: [Uranus Opposition] </t>
   </si>
   <si>
     <t>33</t>
@@ -121,7 +106,7 @@
     <t>3 Taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">33: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 34: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 35: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">34: [Neptune Quincunx] </t>
   </si>
   <si>
     <t>36</t>
@@ -133,16 +118,13 @@
     <t xml:space="preserve">6: [Mars] </t>
   </si>
   <si>
-    <t xml:space="preserve">36: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 37: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 38: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>39</t>
   </si>
   <si>
     <t>9 Taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">39: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 40: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 41: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">41: [Moon Opposition Jupiter Square] </t>
   </si>
   <si>
     <t>42</t>
@@ -151,16 +133,13 @@
     <t>12 Taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">42: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 43: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 44: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>45</t>
   </si>
   <si>
     <t>15 Taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">45: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 46: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 47: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">46: [Mars Conj] </t>
   </si>
   <si>
     <t>48</t>
@@ -169,25 +148,19 @@
     <t>18 Taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">48: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 49: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 50: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>51</t>
   </si>
   <si>
     <t>21 Taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">51: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 52: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 53: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>54</t>
   </si>
   <si>
     <t>24 Taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">54: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 55: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 56: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">54: [Neptune Opposition] 55: [Jupiter Trine] </t>
   </si>
   <si>
     <t>57</t>
@@ -196,34 +169,25 @@
     <t>27 Taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">57: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 58: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 59: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>60</t>
   </si>
   <si>
     <t>0 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">60: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 61: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 62: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>63</t>
   </si>
   <si>
     <t>3 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">63: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 64: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 65: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>66</t>
   </si>
   <si>
     <t>6 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">66: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 67: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 68: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">66: [Mars Semisextile] </t>
   </si>
   <si>
     <t>69</t>
@@ -232,7 +196,7 @@
     <t>9 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">69: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 70: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 71: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">71: [Jupiter Trine] </t>
   </si>
   <si>
     <t>72</t>
@@ -241,7 +205,7 @@
     <t>12 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">72: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 73: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 74: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">74: [Neptune Opposition] </t>
   </si>
   <si>
     <t>75</t>
@@ -250,25 +214,19 @@
     <t>15 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">75: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 76: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 77: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>78</t>
   </si>
   <si>
     <t>18 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">78: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 79: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 80: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>81</t>
   </si>
   <si>
     <t>21 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">81: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 82: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 83: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">82: [Saturn Conj] </t>
   </si>
   <si>
     <t>84</t>
@@ -277,18 +235,12 @@
     <t>24 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">84: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 85: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 86: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>87</t>
   </si>
   <si>
     <t>27 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">87: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 88: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 89: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>90</t>
   </si>
   <si>
@@ -298,7 +250,7 @@
     <t xml:space="preserve">2: [Saturn] </t>
   </si>
   <si>
-    <t xml:space="preserve">90: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 91: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 92: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">90: [Mars Sextile] </t>
   </si>
   <si>
     <t>93</t>
@@ -307,7 +259,7 @@
     <t>3 Cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">93: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 94: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 95: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">93: [Jupiter Quincunx] </t>
   </si>
   <si>
     <t>96</t>
@@ -316,25 +268,19 @@
     <t>6 Cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">96: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 97: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 98: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>99</t>
   </si>
   <si>
     <t>9 Cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">99: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 100: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 101: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>102</t>
   </si>
   <si>
     <t>12 Cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">102: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 103: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 104: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">102: [Mars Sextile Saturn Conj] </t>
   </si>
   <si>
     <t>105</t>
@@ -343,25 +289,19 @@
     <t>15 Cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">105: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 106: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 107: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>108</t>
   </si>
   <si>
     <t>18 Cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">108: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 109: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 110: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>111</t>
   </si>
   <si>
     <t>21 Cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">111: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 112: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 113: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">113: [Jupiter Opposition] </t>
   </si>
   <si>
     <t>114</t>
@@ -370,16 +310,13 @@
     <t>24 Cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">114: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 115: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 116: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>117</t>
   </si>
   <si>
     <t>27 Cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">117: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 118: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 119: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">118: [Mars Square] </t>
   </si>
   <si>
     <t>120</t>
@@ -388,7 +325,7 @@
     <t>0 Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">120: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 121: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 122: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">122: [Saturn Semisextile] </t>
   </si>
   <si>
     <t>123</t>
@@ -397,16 +334,13 @@
     <t>3 Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">123: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 124: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 125: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>126</t>
   </si>
   <si>
     <t>6 Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">126: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 127: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 128: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">128: [Asc Conj] </t>
   </si>
   <si>
     <t>129</t>
@@ -415,16 +349,13 @@
     <t>9 Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">129: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 130: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 131: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>132</t>
   </si>
   <si>
     <t>12 Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">132: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 133: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 134: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">133: [Jupiter Opposition] 134: [Mars Square] </t>
   </si>
   <si>
     <t>135</t>
@@ -436,34 +367,25 @@
     <t xml:space="preserve">17: [Asc] </t>
   </si>
   <si>
-    <t xml:space="preserve">135: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 136: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 137: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>138</t>
   </si>
   <si>
     <t>18 Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">138: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 139: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 140: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>141</t>
   </si>
   <si>
     <t>21 Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">141: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 142: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 143: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>144</t>
   </si>
   <si>
     <t>24 Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">144: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 145: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 146: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">146: [Asc Conj Saturn Sextile] </t>
   </si>
   <si>
     <t>147</t>
@@ -472,7 +394,7 @@
     <t>27 Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">147: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 148: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 149: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">147: [Mercury Conj] 148: [Mars Trine] 149: [Sun Conj] </t>
   </si>
   <si>
     <t>150</t>
@@ -481,18 +403,12 @@
     <t>0 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">150: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 151: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 152: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>153</t>
   </si>
   <si>
     <t>3 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">153: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 154: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 155: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>156</t>
   </si>
   <si>
@@ -502,7 +418,7 @@
     <t xml:space="preserve">7: [Mercury] 8: [Sun] </t>
   </si>
   <si>
-    <t xml:space="preserve">156: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 157: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 158: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">158: [Asc Semisextile Saturn Sextile] </t>
   </si>
   <si>
     <t>159</t>
@@ -511,16 +427,13 @@
     <t>9 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">159: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 160: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 161: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>162</t>
   </si>
   <si>
     <t>12 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">162: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 163: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 164: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">164: [Mars Trine] </t>
   </si>
   <si>
     <t>165</t>
@@ -529,7 +442,7 @@
     <t>15 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">165: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 166: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 167: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">167: [Sun Conj Mercury Conj] </t>
   </si>
   <si>
     <t>168</t>
@@ -538,16 +451,13 @@
     <t>18 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">168: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 169: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 170: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>171</t>
   </si>
   <si>
     <t>21 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">171: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 172: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 173: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">173: [Pluto Conj] </t>
   </si>
   <si>
     <t>174</t>
@@ -556,7 +466,7 @@
     <t>24 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">174: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 175: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 176: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">174: [Saturn Square] 176: [Asc Semisextile] </t>
   </si>
   <si>
     <t>177</t>
@@ -565,7 +475,7 @@
     <t>27 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">177: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 178: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 179: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">179: [Sun Semisextile] </t>
   </si>
   <si>
     <t>180</t>
@@ -574,9 +484,6 @@
     <t>0 Libra</t>
   </si>
   <si>
-    <t xml:space="preserve">180: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 181: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 182: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>183</t>
   </si>
   <si>
@@ -586,7 +493,7 @@
     <t xml:space="preserve">3: [Pluto] </t>
   </si>
   <si>
-    <t xml:space="preserve">183: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 184: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 185: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">185: [Venus Conj] </t>
   </si>
   <si>
     <t>186</t>
@@ -595,7 +502,7 @@
     <t>6 Libra</t>
   </si>
   <si>
-    <t xml:space="preserve">186: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 187: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 188: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">186: [Mars Quincunx] 187: [Mercury Semisextile] 188: [Asc Sextile] </t>
   </si>
   <si>
     <t>189</t>
@@ -604,7 +511,7 @@
     <t>9 Libra</t>
   </si>
   <si>
-    <t xml:space="preserve">189: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 190: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 191: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">190: [Saturn Square Uranus Conj] </t>
   </si>
   <si>
     <t>192</t>
@@ -613,7 +520,7 @@
     <t>12 Libra</t>
   </si>
   <si>
-    <t xml:space="preserve">192: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 193: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 194: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">193: [Pluto Conj] </t>
   </si>
   <si>
     <t>195</t>
@@ -625,7 +532,7 @@
     <t xml:space="preserve">15: [Venus] </t>
   </si>
   <si>
-    <t xml:space="preserve">195: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 196: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 197: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">197: [Sun Semisextile] </t>
   </si>
   <si>
     <t>198</t>
@@ -637,16 +544,13 @@
     <t xml:space="preserve">20: [Uranus] </t>
   </si>
   <si>
-    <t xml:space="preserve">198: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 199: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 200: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>201</t>
   </si>
   <si>
     <t>21 Libra</t>
   </si>
   <si>
-    <t xml:space="preserve">201: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 202: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 203: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">203: [Moon Conj] </t>
   </si>
   <si>
     <t>204</t>
@@ -655,7 +559,7 @@
     <t>24 Libra</t>
   </si>
   <si>
-    <t xml:space="preserve">204: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 205: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 206: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">204: [Saturn Trine] 205: [Venus Conj] 206: [Asc Sextile Mars Opposition] </t>
   </si>
   <si>
     <t>207</t>
@@ -664,7 +568,7 @@
     <t>27 Libra</t>
   </si>
   <si>
-    <t xml:space="preserve">207: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 208: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 209: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">209: [Sun Sextile] </t>
   </si>
   <si>
     <t>210</t>
@@ -676,7 +580,7 @@
     <t xml:space="preserve">2: [Moon] </t>
   </si>
   <si>
-    <t xml:space="preserve">210: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 211: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 212: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">210: [Uranus Conj] 211: [Mercury Sextile] </t>
   </si>
   <si>
     <t>213</t>
@@ -685,7 +589,7 @@
     <t>3 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">213: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 214: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 215: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">213: [Pluto Semisextile] </t>
   </si>
   <si>
     <t>216</t>
@@ -694,7 +598,7 @@
     <t>6 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">216: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 217: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 218: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">218: [Asc Square] </t>
   </si>
   <si>
     <t>219</t>
@@ -703,7 +607,7 @@
     <t>9 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">219: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 220: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 221: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">220: [Saturn Trine] 221: [Moon Conj] </t>
   </si>
   <si>
     <t>222</t>
@@ -712,7 +616,7 @@
     <t>12 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">222: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 223: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 224: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">223: [Mercury Sextile] </t>
   </si>
   <si>
     <t>225</t>
@@ -721,7 +625,7 @@
     <t>15 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">225: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 226: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 227: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">225: [Venus Semisextile] 226: [Mars Opposition] 227: [Sun Sextile] </t>
   </si>
   <si>
     <t>228</t>
@@ -730,7 +634,7 @@
     <t>18 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">228: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 229: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 230: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">230: [Uranus Semisextile] </t>
   </si>
   <si>
     <t>231</t>
@@ -739,7 +643,7 @@
     <t>21 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">231: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 232: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 233: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">233: [Moon Semisextile] </t>
   </si>
   <si>
     <t>234</t>
@@ -748,7 +652,7 @@
     <t>24 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">234: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 235: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 236: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">234: [Neptune Conj] 236: [Asc Square] </t>
   </si>
   <si>
     <t>237</t>
@@ -757,7 +661,7 @@
     <t>27 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">237: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 238: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 239: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">237: [Pluto Sextile] 239: [Sun Square Mercury Square] </t>
   </si>
   <si>
     <t>240</t>
@@ -766,7 +670,7 @@
     <t>0 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">240: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 241: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 242: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">242: [Saturn Quincunx] </t>
   </si>
   <si>
     <t>243</t>
@@ -778,16 +682,13 @@
     <t xml:space="preserve">4: [Neptune] </t>
   </si>
   <si>
-    <t xml:space="preserve">243: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 244: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 245: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>246</t>
   </si>
   <si>
     <t>6 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">246: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 247: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 248: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">248: [Asc Trine] </t>
   </si>
   <si>
     <t>249</t>
@@ -796,7 +697,7 @@
     <t>9 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">249: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 250: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 251: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">249: [Venus Sextile Pluto Sextile] 251: [Moon Semisextile] </t>
   </si>
   <si>
     <t>252</t>
@@ -805,7 +706,7 @@
     <t>12 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">252: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 253: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 254: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">254: [Uranus Sextile Neptune Conj] </t>
   </si>
   <si>
     <t>255</t>
@@ -814,7 +715,7 @@
     <t>15 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">255: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 256: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 257: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">255: [Mercury Square] 257: [Sun Square] </t>
   </si>
   <si>
     <t>258</t>
@@ -823,16 +724,13 @@
     <t>18 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">258: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 259: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 260: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>261</t>
   </si>
   <si>
     <t>21 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">261: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 262: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 263: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">261: [Venus Sextile] 262: [Saturn Opposition] 263: [Moon Sextile] </t>
   </si>
   <si>
     <t>264</t>
@@ -841,7 +739,7 @@
     <t>24 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">264: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 265: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 266: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">265: [Pluto Square] 266: [Asc Trine Uranus Sextile] </t>
   </si>
   <si>
     <t>267</t>
@@ -850,7 +748,7 @@
     <t>27 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">267: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 268: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 269: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">269: [Sun Trine Mercury Trine] </t>
   </si>
   <si>
     <t>270</t>
@@ -859,16 +757,13 @@
     <t>0 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">270: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 271: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 272: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>273</t>
   </si>
   <si>
     <t>3 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">273: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 274: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 275: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">274: [Neptune Semisextile] </t>
   </si>
   <si>
     <t>276</t>
@@ -877,7 +772,7 @@
     <t>6 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">276: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 277: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 278: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">277: [Venus Square] 278: [Asc Quincunx] </t>
   </si>
   <si>
     <t>279</t>
@@ -886,7 +781,7 @@
     <t>9 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">279: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 280: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 281: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">281: [Moon Sextile Pluto Square] </t>
   </si>
   <si>
     <t>282</t>
@@ -895,7 +790,7 @@
     <t>12 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">282: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 283: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 284: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">282: [Saturn Opposition Uranus Square] </t>
   </si>
   <si>
     <t>285</t>
@@ -904,7 +799,7 @@
     <t>15 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">285: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 286: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 287: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">285: [Mercury Trine] 287: [Sun Trine] </t>
   </si>
   <si>
     <t>288</t>
@@ -913,16 +808,13 @@
     <t>18 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">288: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 289: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 290: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>291</t>
   </si>
   <si>
     <t>21 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">291: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 292: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 293: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">293: [Moon Square Venus Square Jupiter Conj] </t>
   </si>
   <si>
     <t>294</t>
@@ -931,7 +823,7 @@
     <t>24 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">294: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 295: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 296: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">295: [Pluto Trine] 296: [Asc Quincunx] </t>
   </si>
   <si>
     <t>297</t>
@@ -940,7 +832,7 @@
     <t>27 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">297: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 298: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 299: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">298: [Uranus Square Neptune Sextile] 299: [Sun Quincunx] </t>
   </si>
   <si>
     <t>300</t>
@@ -949,9 +841,6 @@
     <t>0 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">300: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 301: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 302: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>303</t>
   </si>
   <si>
@@ -961,16 +850,13 @@
     <t xml:space="preserve">3: [Jupiter] </t>
   </si>
   <si>
-    <t xml:space="preserve">303: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 304: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 305: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>306</t>
   </si>
   <si>
     <t>6 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">306: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 307: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 308: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">307: [Mercury Quincunx Venus Trine] 308: [Asc Opposition] </t>
   </si>
   <si>
     <t>309</t>
@@ -979,7 +865,7 @@
     <t>9 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">309: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 310: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 311: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">310: [Neptune Sextile] 311: [Moon Square Pluto Trine] </t>
   </si>
   <si>
     <t>312</t>
@@ -988,7 +874,7 @@
     <t>12 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">312: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 313: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 314: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">312: [Uranus Trine] 313: [Jupiter Conj] </t>
   </si>
   <si>
     <t>315</t>
@@ -997,7 +883,7 @@
     <t>15 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">315: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 316: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 317: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">317: [Sun Quincunx] </t>
   </si>
   <si>
     <t>318</t>
@@ -1006,16 +892,13 @@
     <t>18 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">318: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 319: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 320: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>321</t>
   </si>
   <si>
     <t>21 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">321: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 322: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 323: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">323: [Moon Trine Venus Trine] </t>
   </si>
   <si>
     <t>324</t>
@@ -1024,7 +907,7 @@
     <t>24 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">324: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 325: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 326: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">326: [Asc Opposition Neptune Square] </t>
   </si>
   <si>
     <t>327</t>
@@ -1033,7 +916,7 @@
     <t>27 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">327: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 328: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 329: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">327: [Mercury Opposition] 328: [Uranus Trine] 329: [Sun Opposition] </t>
   </si>
   <si>
     <t>330</t>
@@ -1042,16 +925,13 @@
     <t>0 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">330: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 331: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 332: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>333</t>
   </si>
   <si>
     <t>3 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">333: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 334: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 335: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">333: [Jupiter Semisextile Pluto Quincunx] </t>
   </si>
   <si>
     <t>336</t>
@@ -1060,16 +940,13 @@
     <t>6 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">336: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 337: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 338: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
-  </si>
-  <si>
     <t>339</t>
   </si>
   <si>
     <t>9 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">339: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 340: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 341: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">341: [Moon Trine] </t>
   </si>
   <si>
     <t>342</t>
@@ -1078,7 +955,7 @@
     <t>12 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">342: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 343: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 344: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">342: [Neptune Square] </t>
   </si>
   <si>
     <t>345</t>
@@ -1087,7 +964,7 @@
     <t>15 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">345: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 346: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 347: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">345: [Venus Quincunx] 347: [Sun Opposition Mercury Opposition] </t>
   </si>
   <si>
     <t>348</t>
@@ -1096,7 +973,7 @@
     <t>18 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">348: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 349: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 350: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">350: [Uranus Quincunx] </t>
   </si>
   <si>
     <t>351</t>
@@ -1105,7 +982,7 @@
     <t>21 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">351: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 352: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 353: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">353: [Moon Quincunx Pluto Opposition] </t>
   </si>
   <si>
     <t>354</t>
@@ -1114,7 +991,7 @@
     <t>24 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">354: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 355: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 356: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">356: [Neptune Trine] </t>
   </si>
   <si>
     <t>357</t>
@@ -1123,7 +1000,7 @@
     <t>27 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">357: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 358: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] 359: [Sun Moon Asc Mercury Venus Mars Jupiter Saturn Uranus Neptune Pluto] </t>
+    <t xml:space="preserve">357: [Jupiter Sextile] </t>
   </si>
 </sst>
 </file>
@@ -1465,9 +1342,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -1477,1311 +1351,1206 @@
     </row>
     <row r="2" spans="2:4">
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="2:4">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" t="s">
-        <v>60</v>
-      </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" t="s">
-        <v>66</v>
-      </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" t="s">
-        <v>78</v>
-      </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" t="s">
-        <v>81</v>
-      </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29" t="s">
-        <v>87</v>
-      </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" t="s">
-        <v>90</v>
-      </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" t="s">
-        <v>100</v>
-      </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" t="s">
-        <v>103</v>
-      </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" t="s">
-        <v>109</v>
-      </c>
       <c r="C36" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" t="s">
-        <v>112</v>
-      </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D38" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="2:4">
-      <c r="B39" t="s">
-        <v>118</v>
-      </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="D40" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D41" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="2:4">
-      <c r="B42" t="s">
-        <v>127</v>
-      </c>
       <c r="C42" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="D42" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="D43" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="2:4">
-      <c r="B44" t="s">
-        <v>133</v>
-      </c>
       <c r="C44" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="B45" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="D46" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="2:4">
-      <c r="B47" t="s">
-        <v>143</v>
-      </c>
       <c r="C47" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="D47" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="2:4">
-      <c r="B48" t="s">
-        <v>146</v>
-      </c>
       <c r="C48" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="D48" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="C49" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="D49" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="C50" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="D50" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51" t="s">
-        <v>155</v>
-      </c>
       <c r="C51" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="D51" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="2:4">
-      <c r="B52" t="s">
-        <v>158</v>
-      </c>
       <c r="C52" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="D52" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="C53" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="D53" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="2:4">
-      <c r="B54" t="s">
-        <v>165</v>
-      </c>
       <c r="C54" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="D54" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="2:4">
       <c r="B55" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="B56" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="C56" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="D56" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="2:4">
-      <c r="B57" t="s">
-        <v>174</v>
-      </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="D57" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="B58" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="C58" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="D58" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="C59" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="D59" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="B60" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="C60" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="D60" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="2:4">
-      <c r="B61" t="s">
-        <v>186</v>
-      </c>
       <c r="C61" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="D61" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="B62" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="C62" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="D62" t="s">
-        <v>187</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="B63" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
       <c r="C63" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="D63" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" t="s">
-        <v>196</v>
+        <v>165</v>
       </c>
       <c r="C64" t="s">
-        <v>195</v>
+        <v>164</v>
       </c>
       <c r="D64" t="s">
-        <v>194</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="2:4">
       <c r="B65" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="C65" t="s">
-        <v>198</v>
+        <v>167</v>
       </c>
       <c r="D65" t="s">
-        <v>197</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="B66" t="s">
-        <v>203</v>
+        <v>172</v>
       </c>
       <c r="C66" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="D66" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
     </row>
     <row r="67" spans="2:4">
       <c r="B67" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="C67" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
       <c r="D67" t="s">
-        <v>204</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="B68" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
       <c r="C68" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="D68" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
     </row>
     <row r="69" spans="2:4">
       <c r="B69" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="C69" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="D69" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="B70" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="C70" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="D70" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="B71" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="C71" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="D71" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="B72" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="C72" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="D72" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="2:4">
       <c r="B73" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="C73" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="D73" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="2:4">
       <c r="B74" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="C74" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="D74" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="B75" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="C75" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="D75" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="B76" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="C76" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="D76" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="B77" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="C77" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="D77" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="2:4">
       <c r="B78" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="C78" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="D78" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
     </row>
     <row r="79" spans="2:4">
       <c r="B79" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="C79" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
       <c r="D79" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="B80" t="s">
-        <v>247</v>
+        <v>215</v>
       </c>
       <c r="C80" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="D80" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
     </row>
     <row r="81" spans="2:4">
       <c r="B81" t="s">
-        <v>250</v>
+        <v>218</v>
       </c>
       <c r="C81" t="s">
-        <v>249</v>
+        <v>217</v>
       </c>
       <c r="D81" t="s">
-        <v>248</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="2:4">
       <c r="B82" t="s">
-        <v>254</v>
+        <v>221</v>
       </c>
       <c r="C82" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
       <c r="D82" t="s">
-        <v>251</v>
+        <v>219</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="B83" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="C83" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
       <c r="D83" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="B84" t="s">
-        <v>260</v>
+        <v>227</v>
       </c>
       <c r="C84" t="s">
-        <v>259</v>
+        <v>226</v>
       </c>
       <c r="D84" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
     </row>
     <row r="85" spans="2:4">
       <c r="B85" t="s">
-        <v>263</v>
+        <v>230</v>
       </c>
       <c r="C85" t="s">
-        <v>262</v>
+        <v>229</v>
       </c>
       <c r="D85" t="s">
-        <v>261</v>
+        <v>228</v>
       </c>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" t="s">
-        <v>266</v>
+        <v>233</v>
       </c>
       <c r="C86" t="s">
-        <v>265</v>
+        <v>232</v>
       </c>
       <c r="D86" t="s">
-        <v>264</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" spans="2:4">
-      <c r="B87" t="s">
-        <v>269</v>
-      </c>
       <c r="C87" t="s">
-        <v>268</v>
+        <v>235</v>
       </c>
       <c r="D87" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
     </row>
     <row r="88" spans="2:4">
       <c r="B88" t="s">
-        <v>272</v>
+        <v>238</v>
       </c>
       <c r="C88" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
       <c r="D88" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" spans="2:4">
       <c r="B89" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="C89" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="D89" t="s">
-        <v>273</v>
+        <v>239</v>
       </c>
     </row>
     <row r="90" spans="2:4">
       <c r="B90" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="C90" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="D90" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
     </row>
     <row r="91" spans="2:4">
-      <c r="B91" t="s">
-        <v>281</v>
-      </c>
       <c r="C91" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
       <c r="D91" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="B92" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="C92" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="D92" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
     </row>
     <row r="93" spans="2:4">
       <c r="B93" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
       <c r="C93" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="D93" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
     </row>
     <row r="94" spans="2:4">
       <c r="B94" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="C94" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="D94" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
     </row>
     <row r="95" spans="2:4">
       <c r="B95" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="C95" t="s">
-        <v>292</v>
+        <v>257</v>
       </c>
       <c r="D95" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
     </row>
     <row r="96" spans="2:4">
       <c r="B96" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
       <c r="C96" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="D96" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="2:4">
-      <c r="B97" t="s">
-        <v>299</v>
-      </c>
       <c r="C97" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
       <c r="D97" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
     </row>
     <row r="98" spans="2:4">
       <c r="B98" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="C98" t="s">
-        <v>301</v>
+        <v>265</v>
       </c>
       <c r="D98" t="s">
-        <v>300</v>
+        <v>264</v>
       </c>
     </row>
     <row r="99" spans="2:4">
       <c r="B99" t="s">
-        <v>305</v>
+        <v>269</v>
       </c>
       <c r="C99" t="s">
-        <v>304</v>
+        <v>268</v>
       </c>
       <c r="D99" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
     </row>
     <row r="100" spans="2:4">
       <c r="B100" t="s">
-        <v>308</v>
+        <v>272</v>
       </c>
       <c r="C100" t="s">
-        <v>307</v>
+        <v>271</v>
       </c>
       <c r="D100" t="s">
-        <v>306</v>
+        <v>270</v>
       </c>
     </row>
     <row r="101" spans="2:4">
-      <c r="B101" t="s">
-        <v>311</v>
-      </c>
       <c r="C101" t="s">
-        <v>310</v>
+        <v>274</v>
       </c>
       <c r="D101" t="s">
-        <v>309</v>
+        <v>273</v>
       </c>
     </row>
     <row r="102" spans="2:4">
       <c r="B102" t="s">
-        <v>315</v>
+        <v>277</v>
       </c>
       <c r="C102" t="s">
-        <v>313</v>
+        <v>276</v>
       </c>
       <c r="D102" t="s">
-        <v>312</v>
+        <v>275</v>
       </c>
     </row>
     <row r="103" spans="2:4">
       <c r="B103" t="s">
-        <v>318</v>
+        <v>280</v>
       </c>
       <c r="C103" t="s">
-        <v>317</v>
+        <v>279</v>
       </c>
       <c r="D103" t="s">
-        <v>316</v>
+        <v>278</v>
       </c>
     </row>
     <row r="104" spans="2:4">
       <c r="B104" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
       <c r="C104" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="D104" t="s">
-        <v>319</v>
+        <v>281</v>
       </c>
     </row>
     <row r="105" spans="2:4">
       <c r="B105" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="C105" t="s">
-        <v>323</v>
+        <v>285</v>
       </c>
       <c r="D105" t="s">
-        <v>322</v>
+        <v>284</v>
       </c>
     </row>
     <row r="106" spans="2:4">
       <c r="B106" t="s">
-        <v>327</v>
+        <v>289</v>
       </c>
       <c r="C106" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
       <c r="D106" t="s">
-        <v>325</v>
+        <v>287</v>
       </c>
     </row>
     <row r="107" spans="2:4">
-      <c r="B107" t="s">
-        <v>330</v>
-      </c>
       <c r="C107" t="s">
-        <v>329</v>
+        <v>291</v>
       </c>
       <c r="D107" t="s">
-        <v>328</v>
+        <v>290</v>
       </c>
     </row>
     <row r="108" spans="2:4">
       <c r="B108" t="s">
-        <v>333</v>
+        <v>294</v>
       </c>
       <c r="C108" t="s">
-        <v>332</v>
+        <v>293</v>
       </c>
       <c r="D108" t="s">
-        <v>331</v>
+        <v>292</v>
       </c>
     </row>
     <row r="109" spans="2:4">
       <c r="B109" t="s">
-        <v>336</v>
+        <v>297</v>
       </c>
       <c r="C109" t="s">
-        <v>335</v>
+        <v>296</v>
       </c>
       <c r="D109" t="s">
-        <v>334</v>
+        <v>295</v>
       </c>
     </row>
     <row r="110" spans="2:4">
       <c r="B110" t="s">
-        <v>339</v>
+        <v>300</v>
       </c>
       <c r="C110" t="s">
-        <v>338</v>
+        <v>299</v>
       </c>
       <c r="D110" t="s">
-        <v>337</v>
+        <v>298</v>
       </c>
     </row>
     <row r="111" spans="2:4">
-      <c r="B111" t="s">
-        <v>342</v>
-      </c>
       <c r="C111" t="s">
-        <v>341</v>
+        <v>302</v>
       </c>
       <c r="D111" t="s">
-        <v>340</v>
+        <v>301</v>
       </c>
     </row>
     <row r="112" spans="2:4">
       <c r="B112" t="s">
-        <v>345</v>
+        <v>305</v>
       </c>
       <c r="C112" t="s">
-        <v>344</v>
+        <v>304</v>
       </c>
       <c r="D112" t="s">
-        <v>343</v>
+        <v>303</v>
       </c>
     </row>
     <row r="113" spans="2:4">
-      <c r="B113" t="s">
-        <v>348</v>
-      </c>
       <c r="C113" t="s">
-        <v>347</v>
+        <v>307</v>
       </c>
       <c r="D113" t="s">
-        <v>346</v>
+        <v>306</v>
       </c>
     </row>
     <row r="114" spans="2:4">
       <c r="B114" t="s">
-        <v>351</v>
+        <v>310</v>
       </c>
       <c r="C114" t="s">
-        <v>350</v>
+        <v>309</v>
       </c>
       <c r="D114" t="s">
-        <v>349</v>
+        <v>308</v>
       </c>
     </row>
     <row r="115" spans="2:4">
       <c r="B115" t="s">
-        <v>354</v>
+        <v>313</v>
       </c>
       <c r="C115" t="s">
-        <v>353</v>
+        <v>312</v>
       </c>
       <c r="D115" t="s">
-        <v>352</v>
+        <v>311</v>
       </c>
     </row>
     <row r="116" spans="2:4">
       <c r="B116" t="s">
-        <v>357</v>
+        <v>316</v>
       </c>
       <c r="C116" t="s">
-        <v>356</v>
+        <v>315</v>
       </c>
       <c r="D116" t="s">
-        <v>355</v>
+        <v>314</v>
       </c>
     </row>
     <row r="117" spans="2:4">
       <c r="B117" t="s">
-        <v>360</v>
+        <v>319</v>
       </c>
       <c r="C117" t="s">
-        <v>359</v>
+        <v>318</v>
       </c>
       <c r="D117" t="s">
-        <v>358</v>
+        <v>317</v>
       </c>
     </row>
     <row r="118" spans="2:4">
       <c r="B118" t="s">
-        <v>363</v>
+        <v>322</v>
       </c>
       <c r="C118" t="s">
-        <v>362</v>
+        <v>321</v>
       </c>
       <c r="D118" t="s">
-        <v>361</v>
+        <v>320</v>
       </c>
     </row>
     <row r="119" spans="2:4">
       <c r="B119" t="s">
-        <v>366</v>
+        <v>325</v>
       </c>
       <c r="C119" t="s">
-        <v>365</v>
+        <v>324</v>
       </c>
       <c r="D119" t="s">
-        <v>364</v>
+        <v>323</v>
       </c>
     </row>
     <row r="120" spans="2:4">
       <c r="B120" t="s">
-        <v>369</v>
+        <v>328</v>
       </c>
       <c r="C120" t="s">
-        <v>368</v>
+        <v>327</v>
       </c>
       <c r="D120" t="s">
-        <v>367</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added headers to the spreadsheet chart row
</commit_message>
<xml_diff>
--- a/bchart.xlsx
+++ b/bchart.xlsx
@@ -16,6 +16,48 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="329">
   <si>
+    <t>Planet / Orb</t>
+  </si>
+  <si>
+    <t>Degree Sign</t>
+  </si>
+  <si>
+    <t>Degree range start</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>Asc</t>
+  </si>
+  <si>
+    <t>Mercury</t>
+  </si>
+  <si>
+    <t>Venus</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>Jupiter</t>
+  </si>
+  <si>
+    <t>Saturn</t>
+  </si>
+  <si>
+    <t>Uranus</t>
+  </si>
+  <si>
+    <t>Neptune</t>
+  </si>
+  <si>
+    <t>Pluto</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
@@ -43,7 +85,7 @@
     <t>9 Aries</t>
   </si>
   <si>
-    <t xml:space="preserve">9: [Jupiter Sextile] 10: [Uranus Opposition] 11: [Moon Quincunx] </t>
+    <t xml:space="preserve">9: [Jupiter Sextile] 10: [Uranus Opposition] </t>
   </si>
   <si>
     <t>12</t>
@@ -106,9 +148,6 @@
     <t>3 Taurus</t>
   </si>
   <si>
-    <t xml:space="preserve">34: [Neptune Quincunx] </t>
-  </si>
-  <si>
     <t>36</t>
   </si>
   <si>
@@ -187,9 +226,6 @@
     <t>6 Gemini</t>
   </si>
   <si>
-    <t xml:space="preserve">66: [Mars Semisextile] </t>
-  </si>
-  <si>
     <t>69</t>
   </si>
   <si>
@@ -259,9 +295,6 @@
     <t>3 Cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">93: [Jupiter Quincunx] </t>
-  </si>
-  <si>
     <t>96</t>
   </si>
   <si>
@@ -325,9 +358,6 @@
     <t>0 Leo</t>
   </si>
   <si>
-    <t xml:space="preserve">122: [Saturn Semisextile] </t>
-  </si>
-  <si>
     <t>123</t>
   </si>
   <si>
@@ -418,7 +448,7 @@
     <t xml:space="preserve">7: [Mercury] 8: [Sun] </t>
   </si>
   <si>
-    <t xml:space="preserve">158: [Asc Semisextile Saturn Sextile] </t>
+    <t xml:space="preserve">158: [Saturn Sextile] </t>
   </si>
   <si>
     <t>159</t>
@@ -466,7 +496,7 @@
     <t>24 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">174: [Saturn Square] 176: [Asc Semisextile] </t>
+    <t xml:space="preserve">174: [Saturn Square] </t>
   </si>
   <si>
     <t>177</t>
@@ -475,9 +505,6 @@
     <t>27 Virgo</t>
   </si>
   <si>
-    <t xml:space="preserve">179: [Sun Semisextile] </t>
-  </si>
-  <si>
     <t>180</t>
   </si>
   <si>
@@ -502,7 +529,7 @@
     <t>6 Libra</t>
   </si>
   <si>
-    <t xml:space="preserve">186: [Mars Quincunx] 187: [Mercury Semisextile] 188: [Asc Sextile] </t>
+    <t xml:space="preserve">188: [Asc Sextile] </t>
   </si>
   <si>
     <t>189</t>
@@ -532,9 +559,6 @@
     <t xml:space="preserve">15: [Venus] </t>
   </si>
   <si>
-    <t xml:space="preserve">197: [Sun Semisextile] </t>
-  </si>
-  <si>
     <t>198</t>
   </si>
   <si>
@@ -589,9 +613,6 @@
     <t>3 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">213: [Pluto Semisextile] </t>
-  </si>
-  <si>
     <t>216</t>
   </si>
   <si>
@@ -625,7 +646,7 @@
     <t>15 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">225: [Venus Semisextile] 226: [Mars Opposition] 227: [Sun Sextile] </t>
+    <t xml:space="preserve">226: [Mars Opposition] 227: [Sun Sextile] </t>
   </si>
   <si>
     <t>228</t>
@@ -634,18 +655,12 @@
     <t>18 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">230: [Uranus Semisextile] </t>
-  </si>
-  <si>
     <t>231</t>
   </si>
   <si>
     <t>21 Scorpio</t>
   </si>
   <si>
-    <t xml:space="preserve">233: [Moon Semisextile] </t>
-  </si>
-  <si>
     <t>234</t>
   </si>
   <si>
@@ -670,9 +685,6 @@
     <t>0 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">242: [Saturn Quincunx] </t>
-  </si>
-  <si>
     <t>243</t>
   </si>
   <si>
@@ -697,7 +709,7 @@
     <t>9 Sagitarrius</t>
   </si>
   <si>
-    <t xml:space="preserve">249: [Venus Sextile Pluto Sextile] 251: [Moon Semisextile] </t>
+    <t xml:space="preserve">249: [Venus Sextile Pluto Sextile] </t>
   </si>
   <si>
     <t>252</t>
@@ -763,16 +775,13 @@
     <t>3 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">274: [Neptune Semisextile] </t>
-  </si>
-  <si>
     <t>276</t>
   </si>
   <si>
     <t>6 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">277: [Venus Square] 278: [Asc Quincunx] </t>
+    <t xml:space="preserve">277: [Venus Square] </t>
   </si>
   <si>
     <t>279</t>
@@ -823,7 +832,7 @@
     <t>24 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">295: [Pluto Trine] 296: [Asc Quincunx] </t>
+    <t xml:space="preserve">295: [Pluto Trine] </t>
   </si>
   <si>
     <t>297</t>
@@ -832,7 +841,7 @@
     <t>27 Capricorn</t>
   </si>
   <si>
-    <t xml:space="preserve">298: [Uranus Square Neptune Sextile] 299: [Sun Quincunx] </t>
+    <t xml:space="preserve">298: [Uranus Square Neptune Sextile] </t>
   </si>
   <si>
     <t>300</t>
@@ -856,7 +865,7 @@
     <t>6 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">307: [Mercury Quincunx Venus Trine] 308: [Asc Opposition] </t>
+    <t xml:space="preserve">307: [Venus Trine] 308: [Asc Opposition] </t>
   </si>
   <si>
     <t>309</t>
@@ -883,9 +892,6 @@
     <t>15 Aquarius</t>
   </si>
   <si>
-    <t xml:space="preserve">317: [Sun Quincunx] </t>
-  </si>
-  <si>
     <t>318</t>
   </si>
   <si>
@@ -931,9 +937,6 @@
     <t>3 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">333: [Jupiter Semisextile Pluto Quincunx] </t>
-  </si>
-  <si>
     <t>336</t>
   </si>
   <si>
@@ -964,7 +967,7 @@
     <t>15 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">345: [Venus Quincunx] 347: [Sun Opposition Mercury Opposition] </t>
+    <t xml:space="preserve">347: [Sun Opposition Mercury Opposition] </t>
   </si>
   <si>
     <t>348</t>
@@ -973,16 +976,13 @@
     <t>18 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">350: [Uranus Quincunx] </t>
-  </si>
-  <si>
     <t>351</t>
   </si>
   <si>
     <t>21 Pisces</t>
   </si>
   <si>
-    <t xml:space="preserve">353: [Moon Quincunx Pluto Opposition] </t>
+    <t xml:space="preserve">353: [Pluto Opposition] </t>
   </si>
   <si>
     <t>354</t>
@@ -1007,8 +1007,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1036,8 +1044,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1332,943 +1341,946 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D120"/>
+  <dimension ref="B1:O121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="3" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
-      <c r="C1" t="s">
+    <row r="1" spans="2:15">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4">
-      <c r="B2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15">
       <c r="C2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
       <c r="C7" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15">
       <c r="C8" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
       <c r="C11" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
       <c r="B12" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
       <c r="C13" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
       <c r="C16" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="C18" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:4">
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="C21" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="C22" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" t="s">
-        <v>57</v>
-      </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" t="s">
-        <v>60</v>
-      </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="2:4">
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="C27" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" t="s">
-        <v>70</v>
-      </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="2:4">
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="C30" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="C33" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="C34" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" t="s">
-        <v>88</v>
-      </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="2:4">
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="C37" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="2:4">
-      <c r="B38" t="s">
-        <v>95</v>
-      </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="2:4">
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
       <c r="C39" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D39" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40" t="s">
-        <v>100</v>
-      </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="C42" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D42" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="2:4">
-      <c r="B43" t="s">
-        <v>108</v>
-      </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="2:4">
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D44" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="2:4">
-      <c r="B45" t="s">
-        <v>113</v>
-      </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D46" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="2:4">
+      <c r="B47" t="s">
+        <v>126</v>
+      </c>
       <c r="C47" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D47" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="C48" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="D48" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" t="s">
-        <v>123</v>
-      </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D49" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C50" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="2:4">
+      <c r="B51" t="s">
+        <v>136</v>
+      </c>
       <c r="C51" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="D51" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="C52" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="2:4">
-      <c r="B53" t="s">
-        <v>134</v>
-      </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="2:4">
+      <c r="B54" t="s">
+        <v>144</v>
+      </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="2:4">
-      <c r="B55" t="s">
-        <v>139</v>
-      </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="D55" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="B56" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C56" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="D56" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="2:4">
+      <c r="B57" t="s">
+        <v>152</v>
+      </c>
       <c r="C57" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D57" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="2:4">
-      <c r="B58" t="s">
-        <v>147</v>
-      </c>
       <c r="C58" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D58" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C59" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D59" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="B60" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C60" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="D60" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="C61" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="D61" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="2:4">
-      <c r="B62" t="s">
-        <v>159</v>
-      </c>
       <c r="C62" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="D62" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="B63" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C63" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D63" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C64" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D64" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="2:4">
       <c r="B65" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C65" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D65" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="B66" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D66" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="2:4">
       <c r="B67" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C67" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D67" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="B68" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C68" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D68" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="2:4">
       <c r="B69" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C69" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D69" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="B70" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C70" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D70" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="B71" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C71" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D71" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="B72" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C72" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D72" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="2:4">
-      <c r="B73" t="s">
-        <v>194</v>
-      </c>
       <c r="C73" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D73" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="2:4">
       <c r="B74" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C74" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D74" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="B75" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C75" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D75" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="B76" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C76" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D76" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="B77" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C77" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D77" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="78" spans="2:4">
-      <c r="B78" t="s">
-        <v>209</v>
-      </c>
       <c r="C78" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="D78" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="79" spans="2:4">
-      <c r="B79" t="s">
-        <v>212</v>
-      </c>
       <c r="C79" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D79" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="B80" t="s">
+        <v>217</v>
+      </c>
+      <c r="C80" t="s">
+        <v>216</v>
+      </c>
+      <c r="D80" t="s">
         <v>215</v>
-      </c>
-      <c r="C80" t="s">
-        <v>214</v>
-      </c>
-      <c r="D80" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="81" spans="2:4">
       <c r="B81" t="s">
+        <v>220</v>
+      </c>
+      <c r="C81" t="s">
+        <v>219</v>
+      </c>
+      <c r="D81" t="s">
         <v>218</v>
       </c>
-      <c r="C81" t="s">
-        <v>217</v>
-      </c>
-      <c r="D81" t="s">
-        <v>216</v>
-      </c>
     </row>
     <row r="82" spans="2:4">
-      <c r="B82" t="s">
+      <c r="C82" t="s">
+        <v>222</v>
+      </c>
+      <c r="D82" t="s">
         <v>221</v>
-      </c>
-      <c r="C82" t="s">
-        <v>220</v>
-      </c>
-      <c r="D82" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="B83" t="s">
+        <v>225</v>
+      </c>
+      <c r="C83" t="s">
         <v>224</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>223</v>
-      </c>
-      <c r="D83" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="B84" t="s">
+        <v>228</v>
+      </c>
+      <c r="C84" t="s">
         <v>227</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>226</v>
-      </c>
-      <c r="D84" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="85" spans="2:4">
       <c r="B85" t="s">
+        <v>231</v>
+      </c>
+      <c r="C85" t="s">
         <v>230</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>229</v>
-      </c>
-      <c r="D85" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" t="s">
+        <v>234</v>
+      </c>
+      <c r="C86" t="s">
         <v>233</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>232</v>
       </c>
-      <c r="D86" t="s">
-        <v>231</v>
-      </c>
     </row>
     <row r="87" spans="2:4">
+      <c r="B87" t="s">
+        <v>237</v>
+      </c>
       <c r="C87" t="s">
+        <v>236</v>
+      </c>
+      <c r="D87" t="s">
         <v>235</v>
       </c>
-      <c r="D87" t="s">
-        <v>234</v>
-      </c>
     </row>
     <row r="88" spans="2:4">
-      <c r="B88" t="s">
+      <c r="C88" t="s">
+        <v>239</v>
+      </c>
+      <c r="D88" t="s">
         <v>238</v>
-      </c>
-      <c r="C88" t="s">
-        <v>237</v>
-      </c>
-      <c r="D88" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="89" spans="2:4">
       <c r="B89" t="s">
+        <v>242</v>
+      </c>
+      <c r="C89" t="s">
         <v>241</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>240</v>
-      </c>
-      <c r="D89" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="90" spans="2:4">
       <c r="B90" t="s">
+        <v>245</v>
+      </c>
+      <c r="C90" t="s">
         <v>244</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>243</v>
       </c>
-      <c r="D90" t="s">
-        <v>242</v>
-      </c>
     </row>
     <row r="91" spans="2:4">
+      <c r="B91" t="s">
+        <v>248</v>
+      </c>
       <c r="C91" t="s">
+        <v>247</v>
+      </c>
+      <c r="D91" t="s">
         <v>246</v>
       </c>
-      <c r="D91" t="s">
-        <v>245</v>
-      </c>
     </row>
     <row r="92" spans="2:4">
-      <c r="B92" t="s">
+      <c r="C92" t="s">
+        <v>250</v>
+      </c>
+      <c r="D92" t="s">
         <v>249</v>
       </c>
-      <c r="C92" t="s">
-        <v>248</v>
-      </c>
-      <c r="D92" t="s">
-        <v>247</v>
-      </c>
     </row>
     <row r="93" spans="2:4">
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>252</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>251</v>
-      </c>
-      <c r="D93" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="94" spans="2:4">
@@ -2305,6 +2317,9 @@
       </c>
     </row>
     <row r="97" spans="2:4">
+      <c r="B97" t="s">
+        <v>264</v>
+      </c>
       <c r="C97" t="s">
         <v>263</v>
       </c>
@@ -2313,14 +2328,11 @@
       </c>
     </row>
     <row r="98" spans="2:4">
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>266</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>265</v>
-      </c>
-      <c r="D98" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="99" spans="2:4">
@@ -2346,6 +2358,9 @@
       </c>
     </row>
     <row r="101" spans="2:4">
+      <c r="B101" t="s">
+        <v>275</v>
+      </c>
       <c r="C101" t="s">
         <v>274</v>
       </c>
@@ -2354,14 +2369,11 @@
       </c>
     </row>
     <row r="102" spans="2:4">
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>277</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>276</v>
-      </c>
-      <c r="D102" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="103" spans="2:4">
@@ -2417,9 +2429,6 @@
       </c>
     </row>
     <row r="108" spans="2:4">
-      <c r="B108" t="s">
-        <v>294</v>
-      </c>
       <c r="C108" t="s">
         <v>293</v>
       </c>
@@ -2429,38 +2438,38 @@
     </row>
     <row r="109" spans="2:4">
       <c r="B109" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C109" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D109" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="110" spans="2:4">
       <c r="B110" t="s">
+        <v>299</v>
+      </c>
+      <c r="C110" t="s">
+        <v>298</v>
+      </c>
+      <c r="D110" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4">
+      <c r="B111" t="s">
+        <v>302</v>
+      </c>
+      <c r="C111" t="s">
+        <v>301</v>
+      </c>
+      <c r="D111" t="s">
         <v>300</v>
       </c>
-      <c r="C110" t="s">
-        <v>299</v>
-      </c>
-      <c r="D110" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4">
-      <c r="C111" t="s">
-        <v>302</v>
-      </c>
-      <c r="D111" t="s">
-        <v>301</v>
-      </c>
     </row>
     <row r="112" spans="2:4">
-      <c r="B112" t="s">
-        <v>305</v>
-      </c>
       <c r="C112" t="s">
         <v>304</v>
       </c>
@@ -2470,86 +2479,91 @@
     </row>
     <row r="113" spans="2:4">
       <c r="C113" t="s">
+        <v>306</v>
+      </c>
+      <c r="D113" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4">
+      <c r="C114" t="s">
+        <v>308</v>
+      </c>
+      <c r="D114" t="s">
         <v>307</v>
-      </c>
-      <c r="D113" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4">
-      <c r="B114" t="s">
-        <v>310</v>
-      </c>
-      <c r="C114" t="s">
-        <v>309</v>
-      </c>
-      <c r="D114" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="115" spans="2:4">
       <c r="B115" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C115" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D115" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="116" spans="2:4">
       <c r="B116" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C116" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D116" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="117" spans="2:4">
       <c r="B117" t="s">
+        <v>317</v>
+      </c>
+      <c r="C117" t="s">
+        <v>316</v>
+      </c>
+      <c r="D117" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4">
+      <c r="C118" t="s">
         <v>319</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D118" t="s">
         <v>318</v>
-      </c>
-      <c r="D117" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4">
-      <c r="B118" t="s">
-        <v>322</v>
-      </c>
-      <c r="C118" t="s">
-        <v>321</v>
-      </c>
-      <c r="D118" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="119" spans="2:4">
       <c r="B119" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C119" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D119" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="120" spans="2:4">
       <c r="B120" t="s">
+        <v>325</v>
+      </c>
+      <c r="C120" t="s">
+        <v>324</v>
+      </c>
+      <c r="D120" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4">
+      <c r="B121" t="s">
         <v>328</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C121" t="s">
         <v>327</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D121" t="s">
         <v>326</v>
       </c>
     </row>

</xml_diff>